<commit_message>
rimossi pacchetti inutilizzati ed aggiunto diagramma di gantt
</commit_message>
<xml_diff>
--- a/Documento/nostro/DiagammaDiGantt.xlsx
+++ b/Documento/nostro/DiagammaDiGantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CV19_05\Documento\nostro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5610D6AE-EFE8-478A-ABBB-8A6D953D8352}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8204A4-45CE-43A2-A087-6A6853D29A7D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="207" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>ATTIVITÀ</t>
   </si>
@@ -186,7 +186,45 @@
     <t>Unit testing</t>
   </si>
   <si>
-    <t>Giorni a partire dal 12/12/2019</t>
+    <t>GIORNO</t>
+  </si>
+  <si>
+    <t>DATA DI INIZIO EFFETTIVA:</t>
+  </si>
+  <si>
+    <t>DATA DI FINE EFFETTIVA:</t>
+  </si>
+  <si>
+    <t>(Giorno 1)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(Dopo 62 giorni </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="13"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>lavorativi*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>*Sono esclusi Sabato, Domenica e le feste nazionali</t>
   </si>
 </sst>
 </file>
@@ -199,7 +237,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -387,16 +425,23 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
+      <b/>
+      <sz val="13"/>
       <color theme="1" tint="0.24994659260841701"/>
-      <name val="Corbel"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="major"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
+      <b/>
+      <i/>
+      <sz val="13"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -902,7 +947,7 @@
     <xf numFmtId="0" fontId="1" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -972,9 +1017,6 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="16" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -987,9 +1029,6 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="14" xfId="6" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1022,6 +1061,36 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -2257,7 +2326,7 @@
   <dimension ref="B1:BT33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2280,80 +2349,80 @@
       <c r="G1" s="10"/>
     </row>
     <row r="2" spans="2:72" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="20"/>
       <c r="H2"/>
       <c r="J2" s="13"/>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
       <c r="Q2" s="14"/>
-      <c r="R2" s="38" t="s">
+      <c r="R2" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
       <c r="W2" s="22"/>
-      <c r="X2" s="30" t="s">
+      <c r="X2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="29"/>
+      <c r="AA2" s="29"/>
+      <c r="AB2" s="29"/>
+      <c r="AC2" s="29"/>
       <c r="AD2" s="15"/>
-      <c r="AE2" s="30" t="s">
+      <c r="AE2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="31"/>
-      <c r="AH2" s="31"/>
-      <c r="AI2" s="31"/>
-      <c r="AJ2" s="31"/>
-      <c r="AK2" s="32"/>
+      <c r="AF2" s="29"/>
+      <c r="AG2" s="29"/>
+      <c r="AH2" s="29"/>
+      <c r="AI2" s="29"/>
+      <c r="AJ2" s="29"/>
+      <c r="AK2" s="30"/>
       <c r="AL2" s="16"/>
-      <c r="AM2" s="30" t="s">
+      <c r="AM2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="AN2" s="31"/>
-      <c r="AO2" s="31"/>
-      <c r="AP2" s="31"/>
-      <c r="AQ2" s="31"/>
-      <c r="AR2" s="31"/>
-      <c r="AS2" s="31"/>
-      <c r="AT2" s="31"/>
-      <c r="AU2" s="31"/>
-      <c r="AV2" s="31"/>
+      <c r="AN2" s="29"/>
+      <c r="AO2" s="29"/>
+      <c r="AP2" s="29"/>
+      <c r="AQ2" s="29"/>
+      <c r="AR2" s="29"/>
+      <c r="AS2" s="29"/>
+      <c r="AT2" s="29"/>
+      <c r="AU2" s="29"/>
+      <c r="AV2" s="29"/>
     </row>
     <row r="3" spans="2:72" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="35" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="17" t="s">
@@ -2380,12 +2449,12 @@
       <c r="AA3" s="8"/>
     </row>
     <row r="4" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="35"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -2581,204 +2650,204 @@
       <c r="BT4" s="3"/>
     </row>
     <row r="5" spans="2:72" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="24">
         <v>1</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="24">
         <v>3</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="24">
         <v>1</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="24">
         <v>2</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:72" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="24">
         <v>3</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="24">
         <v>5</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="24">
         <v>2</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="24">
         <v>5</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:72" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="24">
         <v>8</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="24">
         <v>7</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="24">
         <v>5</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="24">
         <v>6</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:72" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="24">
         <v>15</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="24">
         <v>7</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="24">
         <v>11</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="24">
         <v>7</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:72" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="24">
         <v>22</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="24">
         <v>4</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="24">
         <v>18</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="24">
         <v>7</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:72" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="24">
         <v>26</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="24">
         <v>7</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="24">
         <v>25</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="24">
         <v>7</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="26">
         <v>1</v>
       </c>
       <c r="X10" s="12"/>
       <c r="AS10" s="21"/>
     </row>
     <row r="11" spans="2:72" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="24">
         <v>33</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="24">
         <v>7</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="24">
         <v>30</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="24">
         <v>7</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:72" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="24">
         <v>40</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="24">
         <v>2</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="24">
         <v>38</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="24">
         <v>3</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:72" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="24">
         <v>42</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="24">
         <v>15</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="24">
         <v>41</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="24">
         <v>15</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:72" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="24">
         <v>22</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="24">
         <v>15</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="24">
         <v>18</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="24">
         <v>19</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="26">
         <v>1</v>
       </c>
       <c r="H14" s="18"/>
@@ -2848,22 +2917,22 @@
       <c r="BT14" s="19"/>
     </row>
     <row r="15" spans="2:72" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="25">
+      <c r="C15" s="24">
         <v>57</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="24">
         <v>7</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="24">
         <v>56</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="24">
         <v>7</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="26">
         <v>1</v>
       </c>
       <c r="H15"/>
@@ -2961,10 +3030,16 @@
       <c r="AA16"/>
     </row>
     <row r="17" spans="2:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17"/>
+      <c r="B17" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="38">
+        <v>43811</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>26</v>
+      </c>
       <c r="F17"/>
       <c r="G17"/>
       <c r="H17"/>
@@ -2989,12 +3064,18 @@
       <c r="AA17"/>
     </row>
     <row r="18" spans="2:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18"/>
-      <c r="F18" s="23"/>
-      <c r="G18"/>
+      <c r="B18" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="40"/>
+      <c r="D18" s="38">
+        <v>43903</v>
+      </c>
+      <c r="E18" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
       <c r="H18"/>
       <c r="I18"/>
       <c r="J18"/>
@@ -3015,15 +3096,17 @@
       <c r="Y18"/>
       <c r="Z18"/>
       <c r="AA18"/>
-      <c r="AT18" s="29"/>
+      <c r="AT18" s="27"/>
     </row>
-    <row r="19" spans="2:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="28"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
+    <row r="19" spans="2:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
       <c r="H19"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -3046,12 +3129,6 @@
       <c r="AA19"/>
     </row>
     <row r="20" spans="2:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
       <c r="H20"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -3438,7 +3515,11 @@
       <c r="AA33"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="B19:G19"/>
     <mergeCell ref="AM2:AV2"/>
     <mergeCell ref="AE2:AK2"/>
     <mergeCell ref="B2:F2"/>

</xml_diff>